<commit_message>
Santosh Amal Joshua - Capstone Project 1 - Luma Magento Application (Updated)
</commit_message>
<xml_diff>
--- a/MagentoProjectV2/src/test/resources/ProjectExcelData.xlsx
+++ b/MagentoProjectV2/src/test/resources/ProjectExcelData.xlsx
@@ -96,10 +96,10 @@
     <t>Tamil Nadu</t>
   </si>
   <si>
-    <t>jeyajosh1234@gmail.com</t>
-  </si>
-  <si>
-    <t>JeyaJosh123456</t>
+    <t>santoshAmal123@gmail.com</t>
+  </si>
+  <si>
+    <t>SantoshAmal123456</t>
   </si>
 </sst>
 </file>
@@ -425,8 +425,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>